<commit_message>
Change the way price differences are calculated and sort the table by largest negative difference
</commit_message>
<xml_diff>
--- a/data/boardgames_bgg_ids.xlsx
+++ b/data/boardgames_bgg_ids.xlsx
@@ -1038,391 +1038,391 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Betrayal Legacy</t>
+          <t>Beyond the Sun</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>240196</v>
+        <v>317985</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Beyond the Sun</t>
+          <t>Bios: Genesis</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>317985</v>
+        <v>98918</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Bios: Genesis</t>
+          <t>Bios: Megafauna (Second Edition)</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>98918</v>
+        <v>221769</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Bios: Megafauna (Second Edition)</t>
+          <t>Black Angel</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>221769</v>
+        <v>230244</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Black Angel</t>
+          <t>Black Fleet</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>230244</v>
+        <v>157403</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Black Fleet</t>
+          <t>Blitzkrieg!: World War Two in 20 Minutes</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>157403</v>
+        <v>258210</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Blitzkrieg!: World War Two in 20 Minutes</t>
+          <t>Blood Rage</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>258210</v>
+        <v>170216</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Blood Rage</t>
+          <t>Books of Time</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>170216</v>
+        <v>372631</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Books of Time</t>
+          <t>Bosk</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>372631</v>
+        <v>252556</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Bosk</t>
+          <t>Brick &amp; Mortar</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>252556</v>
+        <v>257435</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Brick &amp; Mortar</t>
+          <t>Bumúntú</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>257435</v>
+        <v>201006</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Bumúntú</t>
+          <t>Bunny Kingdom</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>201006</v>
+        <v>184921</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Bunny Kingdom</t>
+          <t>Burgle Bros.</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>184921</v>
+        <v>172081</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Burgle Bros.</t>
+          <t>Bärenpark</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>172081</v>
+        <v>219513</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Bärenpark</t>
+          <t>Cacao: Diamante</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>219513</v>
+        <v>231967</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Cacao: Diamante</t>
+          <t>Caesar!: Seize Rome in 20 Minutes!</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>231967</v>
+        <v>338957</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Caesar!: Seize Rome in 20 Minutes!</t>
+          <t>Café</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>338957</v>
+        <v>284936</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Café</t>
+          <t>Call to Adventure</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>284936</v>
+        <v>238992</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Call to Adventure</t>
+          <t>Campy Creatures</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>238992</v>
+        <v>214396</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Campy Creatures</t>
+          <t>Canopy</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>214396</v>
+        <v>295607</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Canopy</t>
+          <t>Canvas</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>295607</v>
+        <v>290236</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Canvas</t>
+          <t>Cape May</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>290236</v>
+        <v>281248</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Cape May</t>
+          <t>Caper: Europe</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>281248</v>
+        <v>328565</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Caper: Europe</t>
+          <t>Captain Sonar: Operation Dragon</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>328565</v>
+        <v>270444</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Captain Sonar: Operation Dragon</t>
+          <t>Captain Sonar: Upgrade One</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>270444</v>
+        <v>218178</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Captain Sonar: Upgrade One</t>
+          <t>Carnival Zombie: 2nd Edition</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>218178</v>
+        <v>275802</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Carnival Zombie: 2nd Edition</t>
+          <t>Carson City</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>275802</v>
+        <v>39938</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Carson City</t>
+          <t>Cartographers</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>39938</v>
+        <v>263918</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Cartographers</t>
+          <t>Cat in the Box: Deluxe Edition</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>263918</v>
+        <v>345972</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Cat in the Box: Deluxe Edition</t>
+          <t>Catacombs &amp; Castles</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>345972</v>
+        <v>194286</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Catacombs &amp; Castles</t>
+          <t>Catacombs (Third Edition)</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>194286</v>
+        <v>195137</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Catacombs (Third Edition)</t>
+          <t>Caylus 1303</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>195137</v>
+        <v>284818</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Caylus 1303</t>
+          <t>Cellulose: A Plant Cell Biology Game</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>284818</v>
+        <v>333372</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Cellulose: A Plant Cell Biology Game</t>
+          <t>Century: Golem Edition</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>333372</v>
+        <v>232832</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Century: Golem Edition</t>
+          <t>Chai</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>232832</v>
+        <v>253185</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Chai</t>
+          <t>Champions of Midgard</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>253185</v>
+        <v>172287</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Champions of Midgard</t>
+          <t>Charterstone</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>172287</v>
+        <v>197376</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Charterstone</t>
+          <t>Chocolate Factory</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>197376</v>
+        <v>240567</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Chocolate Factory</t>
+          <t>Chocolate Factory: Deluxe Edition</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>240567</v>
+        <v>329434</v>
       </c>
     </row>
     <row r="100">

</xml_diff>